<commit_message>
feature: added more datapoints to the excel sheet
</commit_message>
<xml_diff>
--- a/src/barkley/cross_pred_results.xlsx
+++ b/src/barkley/cross_pred_results.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
   <si>
     <t>N</t>
   </si>
@@ -78,12 +78,21 @@
   <si>
     <t>!!!!</t>
   </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>at N</t>
+  </si>
+  <si>
+    <t>patch size</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,8 +147,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,8 +185,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -234,15 +267,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -266,12 +329,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Ausgabe" xfId="2" builtinId="21"/>
     <cellStyle name="Berechnung" xfId="3" builtinId="22"/>
     <cellStyle name="Eingabe" xfId="1" builtinId="20"/>
     <cellStyle name="Erklärender Text" xfId="4" builtinId="53"/>
+    <cellStyle name="Gut" xfId="5" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="6" builtinId="28"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -285,6 +357,942 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tuning!$B$9:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tuning!$I$9:$I$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>7.1359460692025701E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2282128416532605E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.3874565474518099E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3575337309832504E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.7420621709952504E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.3055672000828301E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.6731448658294104E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.08030854306464E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8BC5-43F1-A6AF-A303C2F31FE5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="412710248"/>
+        <c:axId val="412713528"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="412710248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="412713528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="412713528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="412710248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7F3418C-E919-4A40-BD04-83A31F0CF02D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -587,7 +1595,7 @@
   <dimension ref="B1:Y30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="N3" sqref="N2:N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,13 +2420,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.140625" customWidth="1"/>
+    <col min="8" max="8" width="1.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
@@ -1427,236 +2441,490 @@
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
     </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>161</v>
+      </c>
+      <c r="D3" s="2">
+        <v>161</v>
+      </c>
+      <c r="F3" s="2">
+        <v>164</v>
+      </c>
+      <c r="G3" s="2">
+        <v>162</v>
+      </c>
+      <c r="I3" s="2">
+        <v>165</v>
+      </c>
+      <c r="J3" s="2">
+        <v>164</v>
+      </c>
+    </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="I4" s="2">
+        <v>3</v>
+      </c>
+      <c r="J4" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>3</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3">
+        <f>(C4*C5)^2</f>
+        <v>9</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ref="D6:J6" si="0">(D4*D5)^2</f>
+        <v>16</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2">
-        <v>161</v>
-      </c>
-      <c r="C4" s="2">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2">
-        <v>4</v>
-      </c>
+      <c r="C8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="B9" s="2">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2.0036614475297599E-4</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="F9" s="3">
+        <v>1.84916044399639E-4</v>
+      </c>
+      <c r="G9" s="3">
+        <v>8.85820220754192E-4</v>
+      </c>
+      <c r="I9" s="3">
+        <v>7.1359460692025701E-4</v>
+      </c>
+      <c r="J9" s="3">
+        <v>6.5644790106198798E-3</v>
+      </c>
+      <c r="M9" s="5"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="B10" s="2">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.7259991022395901E-4</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="F10" s="3">
+        <v>1.90428883062033E-4</v>
+      </c>
+      <c r="G10" s="3">
+        <v>8.7758800737793301E-4</v>
+      </c>
+      <c r="I10" s="3">
+        <v>7.2282128416532605E-4</v>
+      </c>
+      <c r="J10" s="3">
+        <v>6.7456662713390797E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="11">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1.5535142551917401E-4</v>
+      </c>
+      <c r="D11" s="3">
+        <v>5.1688068525894697E-4</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1.9284956098657499E-4</v>
+      </c>
+      <c r="G11" s="3">
+        <v>8.3430274507303602E-4</v>
+      </c>
+      <c r="I11" s="3">
+        <v>7.3874565474518099E-4</v>
+      </c>
+      <c r="J11" s="3">
+        <v>6.9632965074918497E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="10">
+        <v>40</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1.5718899552127899E-4</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="F12" s="3">
+        <v>1.85722165500422E-4</v>
+      </c>
+      <c r="G12" s="3">
+        <v>9.0225555567159102E-4</v>
+      </c>
+      <c r="I12" s="3">
+        <v>7.3575337309832504E-4</v>
+      </c>
+      <c r="J12" s="3">
+        <v>7.2895078866260796E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="8">
+        <v>50</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1.3452106815218799E-4</v>
+      </c>
+      <c r="D13" s="3">
+        <v>5.0207518622306197E-4</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1.88446500552483E-4</v>
+      </c>
+      <c r="G13" s="3">
+        <v>9.0476578976827799E-4</v>
+      </c>
+      <c r="I13" s="3">
+        <v>7.7420621709952504E-4</v>
+      </c>
+      <c r="J13" s="3">
+        <v>7.5588931123844799E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <v>80</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.21886151473877E-4</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="F14" s="3">
+        <v>1.9642756071637E-4</v>
+      </c>
+      <c r="G14" s="3">
+        <v>9.4639163527661103E-4</v>
+      </c>
+      <c r="I14" s="3">
+        <v>8.3055672000828301E-4</v>
+      </c>
+      <c r="J14" s="3">
+        <v>8.5831162875826903E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="10">
+        <v>100</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1.11094535713608E-4</v>
+      </c>
+      <c r="D15" s="3">
+        <v>4.22752382804717E-4</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1.96316315524402E-4</v>
+      </c>
+      <c r="G15" s="3">
+        <v>9.3644789188070197E-4</v>
+      </c>
+      <c r="I15" s="3">
+        <v>8.6731448658294104E-4</v>
+      </c>
+      <c r="J15" s="3">
+        <v>9.6453580136129802E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="10">
+        <v>150</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1.0825849110478E-4</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3.87558920528481E-4</v>
+      </c>
+      <c r="F16" s="3">
+        <v>2.07794398905504E-4</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1.1109410112274799E-3</v>
+      </c>
+      <c r="I16" s="3">
+        <v>1.08030854306464E-3</v>
+      </c>
+      <c r="J16" s="3">
+        <v>1.1939220768893199E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="10">
+        <v>200</v>
+      </c>
+      <c r="C17" s="9">
+        <v>8.9120388536307905E-5</v>
+      </c>
+      <c r="D17" s="3">
+        <v>3.5962140735352501E-4</v>
+      </c>
+      <c r="F17" s="3">
+        <v>2.0044748236900799E-4</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1.11655251809299E-3</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3">
+        <v>1.54345627637035E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="10">
+        <v>250</v>
+      </c>
+      <c r="C18" s="9">
+        <v>9.2281648691583E-5</v>
+      </c>
+      <c r="D18" s="3">
+        <v>3.5385553357380301E-4</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1.9306506307164201E-4</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1.2069687691740299E-3</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3">
+        <v>1.8739155966606399E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="10">
+        <v>300</v>
+      </c>
+      <c r="C19" s="9">
+        <v>8.5542056306559203E-5</v>
+      </c>
+      <c r="D19" s="3">
+        <v>3.4613499364561002E-4</v>
+      </c>
+      <c r="F19" s="3">
+        <v>2.0044748236900799E-4</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1.2325424397742501E-3</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3">
+        <v>2.2561235104750801E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="10">
+        <v>350</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3">
+        <v>3.5049175970383503E-4</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="10">
+        <v>400</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3">
+        <v>3.3093149088347001E-4</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="10">
+        <v>450</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3">
+        <v>3.2081719733881401E-4</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="10">
+        <v>500</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3">
+        <v>3.13970744165093E-4</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="12">
+        <v>550</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17">
+        <v>3.2666527358556801E-4</v>
+      </c>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="17"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="18">
+        <f>MIN(C9:C24)</f>
+        <v>8.5542056306559203E-5</v>
+      </c>
+      <c r="D25" s="18">
+        <f t="shared" ref="D25:J25" si="1">MIN(D9:D24)</f>
+        <v>3.13970744165093E-4</v>
+      </c>
+      <c r="F25" s="18">
+        <f t="shared" si="1"/>
+        <v>1.84916044399639E-4</v>
+      </c>
+      <c r="G25" s="18">
+        <f>MIN(G9:G24)</f>
+        <v>8.3430274507303602E-4</v>
+      </c>
+      <c r="I25" s="18">
+        <f t="shared" si="1"/>
+        <v>7.1359460692025701E-4</v>
+      </c>
+      <c r="J25" s="18">
+        <f t="shared" si="1"/>
+        <v>6.5644790106198798E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="20">
+        <f>INDEX($B9:$B24, MATCH(MIN(C9:C24), C9:C24, 0))</f>
+        <v>300</v>
+      </c>
+      <c r="D26" s="20">
+        <f>INDEX($B9:$B24, MATCH(MIN(D9:D24), D9:D24, 0))</f>
+        <v>500</v>
+      </c>
+      <c r="F26" s="20">
+        <f>INDEX($B9:$B24, MATCH(MIN(F9:F24), F9:F24, 0))</f>
         <v>10</v>
       </c>
-      <c r="B10" s="3">
-        <v>2.0036614475297599E-4</v>
-      </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>20</v>
-      </c>
-      <c r="B11" s="3">
-        <v>1.7259991022395901E-4</v>
-      </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+      <c r="G26" s="20">
+        <f>INDEX($B9:$B24, MATCH(MIN(G9:G24), G9:G24, 0))</f>
         <v>30</v>
       </c>
-      <c r="B12" s="3">
-        <v>1.5535142551917401E-4</v>
-      </c>
-      <c r="C12" s="3">
-        <v>5.1688068525894697E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
-        <v>40</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1.5718899552127899E-4</v>
-      </c>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>50</v>
-      </c>
-      <c r="B14" s="3">
-        <v>1.3452106815218799E-4</v>
-      </c>
-      <c r="C14" s="3">
-        <v>5.0207518622306197E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>80</v>
-      </c>
-      <c r="B15" s="3">
-        <v>1.21886151473877E-4</v>
-      </c>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>100</v>
-      </c>
-      <c r="B16" s="3">
-        <v>1.11094535713608E-4</v>
-      </c>
-      <c r="C16" s="3">
-        <v>4.22752382804717E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
-        <v>150</v>
-      </c>
-      <c r="B17" s="3">
-        <v>1.0825849110478E-4</v>
-      </c>
-      <c r="C17" s="3">
-        <v>3.87558920528481E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>200</v>
-      </c>
-      <c r="B18" s="9">
-        <v>8.9120388536307905E-5</v>
-      </c>
-      <c r="C18" s="3">
-        <v>3.5962140735352501E-4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
-        <v>250</v>
-      </c>
-      <c r="B19" s="9">
-        <v>9.2281648691583E-5</v>
-      </c>
-      <c r="C19" s="3">
-        <v>3.5385553357380301E-4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
-        <v>300</v>
-      </c>
-      <c r="B20" s="9">
-        <v>8.5542056306559203E-5</v>
-      </c>
-      <c r="C20" s="3">
-        <v>3.4613499364561002E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
-        <v>350</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3">
-        <v>3.5049175970383503E-4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
-        <v>400</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3">
-        <v>3.3093149088347001E-4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
-        <v>450</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3">
-        <v>3.2081719733881401E-4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
-        <v>500</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3">
-        <v>3.13970744165093E-4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="12">
-        <v>550</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3">
-        <v>3.2666527358556801E-4</v>
+      <c r="I26" s="20">
+        <f>INDEX($B9:$B24, MATCH(MIN(I9:I24), I9:I24, 0))</f>
+        <v>10</v>
+      </c>
+      <c r="J26" s="20">
+        <f>INDEX($B9:$B24, MATCH(MIN(J9:J24), J9:J24, 0))</f>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1664,6 +2932,8 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>